<commit_message>
Adicionando resultados do metodo Maximaze Coverage por KM e Minutos.
</commit_message>
<xml_diff>
--- a/Results PET-CT Solver.xlsx
+++ b/Results PET-CT Solver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carol\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\Downloads\projeto_TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{665D7AA3-15B3-46B6-A3EB-94FA8322291C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C27D05F-CA72-4DD8-B532-A8BD8000A626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{4B58F315-A282-41E6-922E-89FC07149514}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{4B58F315-A282-41E6-922E-89FC07149514}"/>
   </bookViews>
   <sheets>
     <sheet name="Maximaze Coverage - km" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
   <si>
     <t>Cidades Candidatas</t>
   </si>
@@ -148,13 +148,43 @@
   </si>
   <si>
     <t>21.3 s</t>
+  </si>
+  <si>
+    <t>22 s</t>
+  </si>
+  <si>
+    <t>21.1 s</t>
+  </si>
+  <si>
+    <t>28.9 s</t>
+  </si>
+  <si>
+    <t>26.6 s</t>
+  </si>
+  <si>
+    <t>13.9 s</t>
+  </si>
+  <si>
+    <t>17.4 s</t>
+  </si>
+  <si>
+    <t>27.6 s</t>
+  </si>
+  <si>
+    <t>22.7 s</t>
+  </si>
+  <si>
+    <t>27.3 s</t>
+  </si>
+  <si>
+    <t>31.8 s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +199,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -499,17 +535,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -540,21 +573,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -585,6 +603,24 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -900,35 +936,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5EDCCC-AA40-40BE-9295-ECB62574820F}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -949,105 +985,152 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>139</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>645</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>92</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>6</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="17">
+        <v>597899</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>122</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>1023</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>85</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="37">
+        <v>2989351</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>184</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>1794</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>100</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>9</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" s="17">
+        <v>4432150</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>112</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>1192</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>60</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="F6" s="17">
+        <v>1558231</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>519</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="10">
         <v>917</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>70</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>7</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="17">
+        <v>7600206</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="10">
+        <f>SUM(B3:B7)</f>
+        <v>1076</v>
+      </c>
+      <c r="C8" s="10">
+        <f>SUM(C3:C7)</f>
+        <v>5571</v>
+      </c>
+      <c r="D8" s="10">
+        <f>SUM(D3:D7)</f>
+        <v>407</v>
+      </c>
+      <c r="E8" s="10">
+        <f>SUM(E3:E7)</f>
+        <v>37</v>
+      </c>
+      <c r="F8" s="25">
+        <f>SUM(F3:F7)</f>
+        <v>17177837</v>
+      </c>
+      <c r="G8" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -1056,38 +1139,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69F02F6-BEBC-4DFA-9A01-2A6A74648F12}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -1103,100 +1186,120 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>139</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>645</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>92</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>6</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" s="17">
+        <v>206854</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>122</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>1023</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>85</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4" s="17">
+        <v>2782378</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>184</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>1794</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>100</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>9</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F5" s="17">
+        <v>4093152</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>112</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>1192</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>60</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
+      <c r="F6" s="17">
+        <v>1158365</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="10">
         <v>519</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="10">
         <v>917</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>70</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>7</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
+      <c r="F7" s="17">
+        <v>7163162</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1210,33 +1313,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C75FE8F9-692E-4BE1-9ABC-F4083CB71513}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -1257,148 +1360,148 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>139</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>645</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>92</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>6</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="17">
         <v>597899</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>122</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>1023</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>85</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <v>2989351</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>184</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>1794</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>100</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>9</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <v>4432150</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>112</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>1192</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>60</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="17">
         <v>1558231</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>519</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>917</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>70</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>7</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="17">
         <v>7600206</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="25">
         <f>SUM(F3:F7)</f>
         <v>17177837</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="P13" s="10"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P13" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1414,195 +1517,195 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="34"/>
-      <c r="B2" s="35" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="26"/>
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="28" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>139</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>645</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>92</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>6</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="17">
         <v>206854</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="14" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>122</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>1023</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>85</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <v>2782378</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>184</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>1794</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>100</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>9</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <v>4093152</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>112</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>1192</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>60</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="17">
         <v>1158365</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>519</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>917</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>70</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>7</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="17">
         <v>7163162</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="25">
         <f>SUM(F3:F7)</f>
         <v>15403911</v>
       </c>
-      <c r="G8" s="32"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="F9" s="32"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1621,185 +1724,185 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="28" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="30" t="s">
+      <c r="G2" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3" s="8">
         <v>139</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="8">
         <v>645</v>
       </c>
-      <c r="D3" s="11">
+      <c r="D3" s="8">
         <v>92</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="8">
         <v>6</v>
       </c>
-      <c r="F3" s="31">
+      <c r="F3" s="23">
         <v>597899</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>122</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>1023</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>85</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <v>2943646</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>184</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>1794</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>100</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>9</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <v>5393473</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>112</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>1192</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>60</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="17">
         <v>1937951</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>519</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>917</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>70</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>7</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="17">
         <v>13640907</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="26" t="s">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="10">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="10">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="25">
         <f>SUM(F3:F7)</f>
         <v>24513876</v>
       </c>
@@ -1822,185 +1925,185 @@
       <selection activeCell="F3" sqref="F3:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.6640625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="23"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="34"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="9">
         <v>139</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="9">
         <v>645</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="9">
         <v>92</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="9">
         <v>6</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="17">
         <v>206854</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="9">
         <v>122</v>
       </c>
-      <c r="C4" s="12">
+      <c r="C4" s="9">
         <v>1023</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="9">
         <v>85</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="9">
         <v>5</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="17">
         <v>2782378</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="9">
         <v>184</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5" s="9">
         <v>1794</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="9">
         <v>100</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="9">
         <v>9</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="17">
         <v>4768491</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="9">
         <v>112</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="9">
         <v>1192</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="9">
         <v>60</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="9">
         <v>10</v>
       </c>
-      <c r="F6" s="20">
+      <c r="F6" s="17">
         <v>1486423</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="15" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="9">
         <v>519</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="9">
         <v>917</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="9">
         <v>70</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="9">
         <v>7</v>
       </c>
-      <c r="F7" s="20">
+      <c r="F7" s="17">
         <v>8002794</v>
       </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="38">
+      <c r="B8" s="30">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="30">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="30">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="30">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="39">
+      <c r="F8" s="31">
         <f>SUM(F3:F7)</f>
         <v>17246940</v>
       </c>

</xml_diff>

<commit_message>
Update Results PET-CT Solver.xlsx
</commit_message>
<xml_diff>
--- a/Results PET-CT Solver.xlsx
+++ b/Results PET-CT Solver.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thiag\Downloads\projeto_TCC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carol\Documents\GitHub\Distribuicao-PET-CT-TCC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C27D05F-CA72-4DD8-B532-A8BD8000A626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6087AEF6-8B8B-4986-A16A-4FAF614A5F84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{4B58F315-A282-41E6-922E-89FC07149514}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B58F315-A282-41E6-922E-89FC07149514}"/>
   </bookViews>
   <sheets>
     <sheet name="Maximaze Coverage - km" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
   <si>
     <t>Cidades Candidatas</t>
   </si>
@@ -144,9 +144,6 @@
     <t>17 s</t>
   </si>
   <si>
-    <t>23.8</t>
-  </si>
-  <si>
     <t>21.3 s</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>31.8 s</t>
+  </si>
+  <si>
+    <t>23.8 s</t>
   </si>
 </sst>
 </file>
@@ -214,7 +214,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -398,134 +398,233 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -535,14 +634,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -556,9 +652,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,34 +668,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -613,13 +709,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -938,193 +1064,193 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5EDCCC-AA40-40BE-9295-ECB62574820F}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>139</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>645</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="23">
         <v>92</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="23">
         <v>6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="37">
         <v>597899</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="48" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>122</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1023</v>
+      </c>
+      <c r="D4" s="6">
+        <v>85</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+      <c r="F4" s="28">
+        <v>2989351</v>
+      </c>
+      <c r="G4" s="35" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9">
-        <v>122</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1023</v>
-      </c>
-      <c r="D4" s="9">
-        <v>85</v>
-      </c>
-      <c r="E4" s="9">
-        <v>5</v>
-      </c>
-      <c r="F4" s="37">
-        <v>2989351</v>
-      </c>
-      <c r="G4" s="14" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>184</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1794</v>
+      </c>
+      <c r="D5" s="6">
+        <v>100</v>
+      </c>
+      <c r="E5" s="6">
+        <v>9</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4432150</v>
+      </c>
+      <c r="G5" s="35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>112</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1192</v>
+      </c>
+      <c r="D6" s="6">
+        <v>60</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1558231</v>
+      </c>
+      <c r="G6" s="35" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6">
+        <v>519</v>
+      </c>
+      <c r="C7" s="6">
+        <v>917</v>
+      </c>
+      <c r="D7" s="6">
+        <v>70</v>
+      </c>
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
-        <v>184</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1794</v>
-      </c>
-      <c r="D5" s="9">
-        <v>100</v>
-      </c>
-      <c r="E5" s="9">
-        <v>9</v>
-      </c>
-      <c r="F5" s="17">
-        <v>4432150</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9">
-        <v>112</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1192</v>
-      </c>
-      <c r="D6" s="9">
-        <v>60</v>
-      </c>
-      <c r="E6" s="9">
-        <v>10</v>
-      </c>
-      <c r="F6" s="17">
-        <v>1558231</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="F7" s="13">
+        <v>7600206</v>
+      </c>
+      <c r="G7" s="36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10">
-        <v>519</v>
-      </c>
-      <c r="C7" s="10">
-        <v>917</v>
-      </c>
-      <c r="D7" s="10">
-        <v>70</v>
-      </c>
-      <c r="E7" s="10">
-        <v>7</v>
-      </c>
-      <c r="F7" s="17">
-        <v>7600206</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="21">
         <f>SUM(F3:F7)</f>
         <v>17177837</v>
       </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1137,175 +1263,202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C69F02F6-BEBC-4DFA-9A01-2A6A74648F12}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>139</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>645</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="23">
         <v>92</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="23">
         <v>6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="37">
         <v>206854</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>122</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1023</v>
+      </c>
+      <c r="D4" s="6">
+        <v>85</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+      <c r="F4" s="13">
+        <v>2782378</v>
+      </c>
+      <c r="G4" s="32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="9">
-        <v>122</v>
-      </c>
-      <c r="C4" s="9">
-        <v>1023</v>
-      </c>
-      <c r="D4" s="9">
-        <v>85</v>
-      </c>
-      <c r="E4" s="9">
-        <v>5</v>
-      </c>
-      <c r="F4" s="17">
-        <v>2782378</v>
-      </c>
-      <c r="G4" s="14" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="6">
+        <v>184</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1794</v>
+      </c>
+      <c r="D5" s="6">
+        <v>100</v>
+      </c>
+      <c r="E5" s="6">
+        <v>9</v>
+      </c>
+      <c r="F5" s="13">
+        <v>4093152</v>
+      </c>
+      <c r="G5" s="32" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6">
+        <v>112</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1192</v>
+      </c>
+      <c r="D6" s="6">
+        <v>60</v>
+      </c>
+      <c r="E6" s="6">
+        <v>10</v>
+      </c>
+      <c r="F6" s="13">
+        <v>1158365</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="6">
+        <v>519</v>
+      </c>
+      <c r="C7" s="6">
+        <v>917</v>
+      </c>
+      <c r="D7" s="6">
+        <v>70</v>
+      </c>
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
-        <v>184</v>
-      </c>
-      <c r="C5" s="9">
-        <v>1794</v>
-      </c>
-      <c r="D5" s="9">
-        <v>100</v>
-      </c>
-      <c r="E5" s="9">
-        <v>9</v>
-      </c>
-      <c r="F5" s="17">
-        <v>4093152</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="9">
-        <v>112</v>
-      </c>
-      <c r="C6" s="9">
-        <v>1192</v>
-      </c>
-      <c r="D6" s="9">
-        <v>60</v>
-      </c>
-      <c r="E6" s="9">
-        <v>10</v>
-      </c>
-      <c r="F6" s="17">
-        <v>1158365</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="10">
-        <v>519</v>
-      </c>
-      <c r="C7" s="10">
-        <v>917</v>
-      </c>
-      <c r="D7" s="10">
-        <v>70</v>
-      </c>
-      <c r="E7" s="10">
-        <v>7</v>
-      </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>7163162</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>41</v>
-      </c>
+      <c r="G7" s="33" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B3:B7)</f>
+        <v>1076</v>
+      </c>
+      <c r="C8" s="7">
+        <f>SUM(C3:C7)</f>
+        <v>5571</v>
+      </c>
+      <c r="D8" s="7">
+        <f>SUM(D3:D7)</f>
+        <v>407</v>
+      </c>
+      <c r="E8" s="7">
+        <f>SUM(E3:E7)</f>
+        <v>37</v>
+      </c>
+      <c r="F8" s="21">
+        <f>SUM(F3:F7)</f>
+        <v>15403911</v>
+      </c>
+      <c r="G8" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1314,194 +1467,194 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>139</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>645</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="23">
         <v>92</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="23">
         <v>6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="37">
         <v>597899</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="G3" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>122</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>1023</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>85</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <v>2989351</v>
       </c>
-      <c r="G4" s="15" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="G4" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>184</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>1794</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>100</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>9</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <v>4432150</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>112</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>1192</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>60</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>10</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <v>1558231</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>519</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>917</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>70</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>7600206</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="21">
         <f>SUM(F3:F7)</f>
         <v>17177837</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P13" s="7"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="P13" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1517,195 +1670,195 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="27" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38"/>
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>139</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>645</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="23">
         <v>92</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="23">
         <v>6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="37">
         <v>206854</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="24" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>122</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>1023</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>85</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <v>2782378</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>184</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>1794</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>100</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>9</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <v>4093152</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>112</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>1192</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>60</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>10</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <v>1158365</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>519</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>917</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>70</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>7163162</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="21">
         <f>SUM(F3:F7)</f>
         <v>15403911</v>
       </c>
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F9" s="24"/>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1721,188 +1874,188 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="5">
         <v>139</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="5">
         <v>645</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="5">
         <v>92</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>6</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="19">
         <v>597899</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>122</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>1023</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>85</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <v>2943646</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>184</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>1794</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>100</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>9</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <v>5393473</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>112</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>1192</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>60</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>10</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <v>1937951</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>519</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>917</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>70</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>13640907</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="7">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="7">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="7">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="25">
+      <c r="F8" s="21">
         <f>SUM(F3:F7)</f>
         <v>24513876</v>
       </c>
@@ -1922,188 +2075,188 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F7"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="34"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="40" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="23">
         <v>139</v>
       </c>
-      <c r="C3" s="9">
+      <c r="C3" s="23">
         <v>645</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="23">
         <v>92</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="23">
         <v>6</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="37">
         <v>206854</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="24" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="6">
         <v>122</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="6">
         <v>1023</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>85</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="6">
         <v>5</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="13">
         <v>2782378</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="11" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="6">
         <v>184</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="6">
         <v>1794</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>100</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <v>9</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="13">
         <v>4768491</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="6">
         <v>112</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>1192</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>60</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="6">
         <v>10</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="13">
         <v>1486423</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="6">
         <v>519</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>917</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>70</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="13">
         <v>8002794</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="26">
         <f>SUM(B3:B7)</f>
         <v>1076</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="26">
         <f>SUM(C3:C7)</f>
         <v>5571</v>
       </c>
-      <c r="D8" s="30">
+      <c r="D8" s="26">
         <f>SUM(D3:D7)</f>
         <v>407</v>
       </c>
-      <c r="E8" s="30">
+      <c r="E8" s="26">
         <f>SUM(E3:E7)</f>
         <v>37</v>
       </c>
-      <c r="F8" s="31">
+      <c r="F8" s="27">
         <f>SUM(F3:F7)</f>
         <v>17246940</v>
       </c>

</xml_diff>